<commit_message>
sps: Extend perf test excel template
Scope: SafeguardSessions/assets/performance_testing/results.xlsx

Even though initial import is different from refresh since data is
fetched twice, it makes sense to record SPS metrics measured during
initial import so that we can compare it to the load during refresh.

A column from the `Measurement` section was missing where we can record
the baseline SPS performance, so that we can compare the load between
data import and just the standard SPS workload.

References: azure #425857
</commit_message>
<xml_diff>
--- a/SafeguardSessions/assets/performance_testing/results.xlsx
+++ b/SafeguardSessions/assets/performance_testing/results.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26815"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="654" documentId="11_5547C5AED75272C0D3A1AFAF3E3FC27ADA863F77" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC66C82B-2F0A-4F15-907D-3DFE9A8DD49F}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddavid\Repos\SafeguardPowerBI\SafeguardSessions\assets\performance_testing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E12C232-D985-4E97-BCA0-51F3ECC956A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28350" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Background</t>
   </si>
@@ -128,9 +133,6 @@
     <t>Avg CPU usage (%)</t>
   </si>
   <si>
-    <t>Not measured</t>
-  </si>
-  <si>
     <t>Max CPU usage (%)</t>
   </si>
   <si>
@@ -171,6 +173,12 @@
   </si>
   <si>
     <t>Pipeline error count</t>
+  </si>
+  <si>
+    <t>Baseline SPS performance</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -180,7 +188,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -378,12 +386,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -404,16 +430,56 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -432,59 +498,29 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -804,10 +840,10 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:E11"/>
+      <selection activeCell="B11" sqref="B11:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
@@ -819,131 +855,131 @@
     <col min="8" max="14" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="35"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="43" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36" t="s">
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="36"/>
-      <c r="L2" s="37"/>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="40" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="42" t="s">
+      <c r="E3" s="27"/>
+      <c r="F3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="24">
+      <c r="H3" s="33"/>
+      <c r="I3" s="36">
         <v>1500000</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="19"/>
+      <c r="K3" s="22"/>
       <c r="L3" s="5">
         <v>750000</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="38"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="19" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="19"/>
+      <c r="K4" s="22"/>
       <c r="L4" s="5">
         <v>750000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="40" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="19" t="s">
+      <c r="E5" s="28"/>
+      <c r="F5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="22"/>
       <c r="I5" s="4">
         <v>1500000</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="19"/>
+      <c r="K5" s="22"/>
       <c r="L5" s="5">
         <v>1500000</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1">
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="19"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="22"/>
       <c r="G6" s="6"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -951,14 +987,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -969,14 +1005,14 @@
       <c r="K7" s="3"/>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -987,454 +1023,628 @@
       <c r="K8" s="3"/>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32" t="s">
+      <c r="E10" s="18"/>
+      <c r="F10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32" t="s">
+      <c r="G10" s="18"/>
+      <c r="H10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32" t="s">
+      <c r="I10" s="18"/>
+      <c r="J10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="32"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="K10" s="18"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="39">
         <v>45159.24355324074</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28">
+      <c r="E11" s="39"/>
+      <c r="F11" s="39">
         <v>45159.24355324074</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28">
+      <c r="G11" s="39"/>
+      <c r="H11" s="39">
         <v>45159.24355324074</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28">
+      <c r="I11" s="39"/>
+      <c r="J11" s="39">
         <v>45159.24355324074</v>
       </c>
-      <c r="I11" s="28"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="K11" s="39"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="42"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="39">
         <v>45159.243877314817</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28">
+      <c r="E12" s="39"/>
+      <c r="F12" s="39">
         <v>45159.243877314817</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28">
+      <c r="G12" s="39"/>
+      <c r="H12" s="39">
         <v>45159.243877314817</v>
       </c>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28">
+      <c r="I12" s="39"/>
+      <c r="J12" s="39">
         <v>45159.243877314817</v>
       </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="15"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="K12" s="39"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="27">
-        <f>B12-B11</f>
+      <c r="B13" s="44"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="38">
+        <f>D12-D11</f>
         <v>3.2407407707069069E-4</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27">
-        <f t="shared" ref="D13" si="0">D12-D11</f>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38">
+        <f t="shared" ref="F13" si="0">F12-F11</f>
         <v>3.2407407707069069E-4</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27">
-        <f t="shared" ref="F13" si="1">F12-F11</f>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38">
+        <f t="shared" ref="H13" si="1">H12-H11</f>
         <v>3.2407407707069069E-4</v>
       </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27">
-        <f t="shared" ref="H13" si="2">H12-H11</f>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38">
+        <f t="shared" ref="J13" si="2">J12-J11</f>
         <v>3.2407407707069069E-4</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="15"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="K13" s="38"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="17">
+        <v>42.8</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17">
+        <v>42.8</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17">
+        <v>42.8</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17">
+        <v>42.8</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17">
+        <v>42.8</v>
+      </c>
+      <c r="K14" s="17"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="26">
-        <v>42.8</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="26">
-        <v>42.8</v>
-      </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="13" t="s">
+      <c r="B15" s="17">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="K15" s="17"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="26">
-        <v>81.400000000000006</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="26">
-        <v>81.400000000000006</v>
-      </c>
-      <c r="I15" s="26"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="13" t="s">
+      <c r="B16" s="17">
+        <v>26.5</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17">
+        <v>26.5</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17">
+        <v>26.5</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17">
+        <v>26.5</v>
+      </c>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17">
+        <v>26.5</v>
+      </c>
+      <c r="K16" s="17"/>
+      <c r="L16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="26">
-        <v>26.5</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="26">
-        <v>26.5</v>
-      </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="13" t="s">
+      <c r="B17" s="17">
+        <v>27.4</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17">
+        <v>27.4</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17">
+        <v>27.4</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17">
+        <v>27.4</v>
+      </c>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17">
+        <v>27.4</v>
+      </c>
+      <c r="K17" s="17"/>
+      <c r="L17" s="14"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="26">
-        <v>27.4</v>
-      </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="26">
-        <v>27.4</v>
-      </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="13" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="14"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="11" t="s">
+      <c r="B19" s="17">
+        <v>3.05</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17">
+        <v>3.05</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17">
+        <v>3.05</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17">
+        <v>3.05</v>
+      </c>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17">
+        <v>3.05</v>
+      </c>
+      <c r="K19" s="17"/>
+      <c r="L19" s="14"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="26">
-        <v>3.05</v>
-      </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="26">
-        <v>3.05</v>
-      </c>
-      <c r="I19" s="26"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="11" t="s">
+      <c r="B20" s="17">
+        <v>1.02</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17">
+        <v>1.02</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17">
+        <v>1.02</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17">
+        <v>1.02</v>
+      </c>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17">
+        <v>1.02</v>
+      </c>
+      <c r="K20" s="17"/>
+      <c r="L20" s="14"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="26">
-        <v>1.02</v>
-      </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="26">
-        <v>1.02</v>
-      </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="10" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="14"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="17">
+        <v>5.27</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17">
+        <v>5.27</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17">
+        <v>5.27</v>
+      </c>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17">
+        <v>5.27</v>
+      </c>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17">
+        <v>5.27</v>
+      </c>
+      <c r="K22" s="17"/>
+      <c r="L22" s="14"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="17">
+        <v>1.61</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17">
+        <v>1.61</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17">
+        <v>1.61</v>
+      </c>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17">
+        <v>1.61</v>
+      </c>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17">
+        <v>1.61</v>
+      </c>
+      <c r="K23" s="17"/>
+      <c r="L23" s="14"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="15"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="26">
-        <v>5.27</v>
-      </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="26">
-        <v>5.27</v>
-      </c>
-      <c r="I22" s="26"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="15"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="26">
-        <v>1.61</v>
-      </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="26">
-        <v>1.61</v>
-      </c>
-      <c r="I23" s="26"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="15"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="10" t="s">
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="14"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="15"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="11" t="s">
+      <c r="B25" s="17">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="K25" s="17"/>
+      <c r="L25" s="14"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="26">
-        <v>0.79700000000000004</v>
-      </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="26">
-        <v>0.79700000000000004</v>
-      </c>
-      <c r="I25" s="26"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="15"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="11" t="s">
+      <c r="B26" s="17">
+        <v>0</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17">
+        <v>0</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17">
+        <v>0</v>
+      </c>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17">
+        <v>0</v>
+      </c>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17">
+        <v>0</v>
+      </c>
+      <c r="K26" s="17"/>
+      <c r="L26" s="14"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="26">
+      <c r="B27" s="17">
+        <v>33.1</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17">
+        <v>33.1</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17">
+        <v>33.1</v>
+      </c>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17">
+        <v>33.1</v>
+      </c>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17">
+        <v>33.1</v>
+      </c>
+      <c r="K27" s="17"/>
+      <c r="L27" s="14"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="17">
+        <v>0.115</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17">
+        <v>0.115</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17">
+        <v>0.115</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17">
+        <v>0.115</v>
+      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17">
+        <v>0.115</v>
+      </c>
+      <c r="K28" s="17"/>
+      <c r="L28" s="14"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="17">
+        <v>45.1</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17">
+        <v>45.1</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17">
+        <v>45.1</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17">
+        <v>45.1</v>
+      </c>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17">
+        <v>45.1</v>
+      </c>
+      <c r="K29" s="17"/>
+      <c r="L29" s="14"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="16">
         <v>0</v>
       </c>
-      <c r="E26" s="26"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="26">
+      <c r="C30" s="16"/>
+      <c r="D30" s="16">
         <v>0</v>
       </c>
-      <c r="I26" s="26"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="15"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="26">
-        <v>33.1</v>
-      </c>
-      <c r="E27" s="26"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="26">
-        <v>33.1</v>
-      </c>
-      <c r="I27" s="26"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="15"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="26">
-        <v>0.115</v>
-      </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="26">
-        <v>0.115</v>
-      </c>
-      <c r="I28" s="26"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="15"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="26">
-        <v>45.1</v>
-      </c>
-      <c r="E29" s="26"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="26">
-        <v>45.1</v>
-      </c>
-      <c r="I29" s="26"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="15"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="29">
+      <c r="E30" s="16"/>
+      <c r="F30" s="16">
         <v>0</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="29">
+      <c r="G30" s="16"/>
+      <c r="H30" s="16">
         <v>0</v>
       </c>
-      <c r="I30" s="29"/>
-      <c r="J30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16">
+        <v>0</v>
+      </c>
       <c r="K30" s="16"/>
-      <c r="L30" s="17"/>
+      <c r="L30" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
+  <mergeCells count="124">
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J4:K4"/>
@@ -1449,82 +1659,42 @@
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B14:C30"/>
-    <mergeCell ref="F14:G30"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B11:C13"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3:C4" r:id="rId1" location="TOPIC-2021538" display="Help: Hardware specifications table" xr:uid="{7A8CD902-7717-4D9E-8E23-2C949694525A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="41f7933d-0400-4b1c-a588-00c817e14f4e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="22b0a55a-e510-419c-a4ee-932afbf3032e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1763,22 +1933,50 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="41f7933d-0400-4b1c-a588-00c817e14f4e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="22b0a55a-e510-419c-a4ee-932afbf3032e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02CC1CB7-773C-43BC-9FE1-E1D2690FF897}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E6C1AD-222C-47C7-89E9-95E0A1337C9A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDCD546B-5D53-432D-A84D-DB63C0EAF4AB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDCD546B-5D53-432D-A84D-DB63C0EAF4AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="22b0a55a-e510-419c-a4ee-932afbf3032e"/>
+    <ds:schemaRef ds:uri="41f7933d-0400-4b1c-a588-00c817e14f4e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E6C1AD-222C-47C7-89E9-95E0A1337C9A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02CC1CB7-773C-43BC-9FE1-E1D2690FF897}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="41f7933d-0400-4b1c-a588-00c817e14f4e"/>
+    <ds:schemaRef ds:uri="22b0a55a-e510-419c-a4ee-932afbf3032e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>